<commit_message>
Added proper gauges to table, also sets edge thickness based on gauge
</commit_message>
<xml_diff>
--- a/tbl/WireLengthTotal.xlsx
+++ b/tbl/WireLengthTotal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="123">
   <si>
     <t xml:space="preserve">Wire</t>
   </si>
@@ -223,15 +223,6 @@
     <t xml:space="preserve">DASH_CAN_L</t>
   </si>
   <si>
-    <t xml:space="preserve">ACCEL_LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WARM_LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEUTRAL_LED</t>
-  </si>
-  <si>
     <t xml:space="preserve">FLEX</t>
   </si>
   <si>
@@ -370,24 +361,15 @@
     <t xml:space="preserve">BRAKE_OVER_TRAVEL-BRAKE_LIGHT</t>
   </si>
   <si>
-    <t xml:space="preserve">20g white</t>
-  </si>
-  <si>
     <t xml:space="preserve">BRAKE_LIGHT</t>
   </si>
   <si>
     <t xml:space="preserve">RECTIFIER-SUPPLY</t>
   </si>
   <si>
-    <t xml:space="preserve">20g red</t>
-  </si>
-  <si>
     <t xml:space="preserve">IGN-CYL_GND</t>
   </si>
   <si>
-    <t xml:space="preserve">20g blue</t>
-  </si>
-  <si>
     <t xml:space="preserve">SERIAL_TX</t>
   </si>
   <si>
@@ -407,9 +389,6 @@
   </si>
   <si>
     <t xml:space="preserve">BRAKE_TRANSPONDER-GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20g yellow</t>
   </si>
 </sst>
 </file>
@@ -518,10 +497,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E79" activeCellId="0" sqref="E79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G67" activeCellId="0" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,8 +594,8 @@
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <f aca="false">SUM(K2:K70)</f>
-        <v>79888.66</v>
+        <f aca="false">SUM(K2:K67)</f>
+        <v>75179.56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,7 +772,7 @@
       </c>
       <c r="Q6" s="1" t="n">
         <f aca="false">CONVERT(Q2,"mm","in")</f>
-        <v>3145.22283464567</v>
+        <v>2959.82519685039</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>4621</v>
@@ -976,7 +955,7 @@
       </c>
       <c r="Q10" s="1" t="n">
         <f aca="false">Q6/12</f>
-        <v>262.101902887139</v>
+        <v>246.652099737533</v>
       </c>
       <c r="R10" s="0" t="n">
         <v>232</v>
@@ -1032,7 +1011,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="0" t="n">
         <f aca="false">(Q10-R10)*12</f>
-        <v>361.222834645668</v>
+        <v>175.825196850395</v>
       </c>
       <c r="U11" s="0" t="s">
         <v>38</v>
@@ -1055,7 +1034,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>2</v>
@@ -1153,7 +1132,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>2</v>
@@ -1182,7 +1161,7 @@
       </c>
       <c r="Q14" s="1" t="n">
         <f aca="false">CONVERT(Q10,"ft","Nmi")</f>
-        <v>0.0431364254859611</v>
+        <v>0.0405937149028078</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,7 +1775,7 @@
         <v>9982</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1820,13 +1799,13 @@
         <v>13</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>63</v>
       </c>
       <c r="P29" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q29" s="1"/>
     </row>
@@ -1839,7 +1818,7 @@
         <v>9982</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1854,35 +1833,35 @@
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1" t="n">
-        <v>1569.7</v>
+        <v>524.56</v>
       </c>
       <c r="L30" s="1" t="n">
-        <v>1589.7</v>
+        <v>524.56</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="P30" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1897,40 +1876,40 @@
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1" t="n">
-        <v>1569.7</v>
+        <v>0</v>
       </c>
       <c r="L31" s="1" t="n">
-        <v>1589.7</v>
+        <v>10</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="P31" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>2</v>
@@ -1940,28 +1919,28 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1" t="n">
-        <v>1569.7</v>
+        <v>1010.96</v>
       </c>
       <c r="L32" s="1" t="n">
-        <v>1589.7</v>
+        <v>1020.96</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="P32" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="n">
@@ -1973,7 +1952,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>2</v>
@@ -1983,19 +1962,19 @@
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="n">
-        <v>524.56</v>
+        <v>992.96</v>
       </c>
       <c r="L33" s="1" t="n">
-        <v>524.56</v>
+        <v>1002.96</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="P33" s="1" t="n">
         <v>1</v>
@@ -2004,7 +1983,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="n">
@@ -2016,7 +1995,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>2</v>
@@ -2026,19 +2005,19 @@
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1" t="n">
-        <v>0</v>
+        <v>63.52</v>
       </c>
       <c r="L34" s="1" t="n">
-        <v>10</v>
+        <v>63.52</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="P34" s="1" t="n">
         <v>1</v>
@@ -2047,7 +2026,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="n">
@@ -2059,7 +2038,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H35" s="1" t="n">
         <v>2</v>
@@ -2069,28 +2048,28 @@
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1" t="n">
-        <v>1010.96</v>
+        <v>63.52</v>
       </c>
       <c r="L35" s="1" t="n">
-        <v>1020.96</v>
+        <v>63.52</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="N35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="P35" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="n">
@@ -2102,7 +2081,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>2</v>
@@ -2112,19 +2091,19 @@
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1" t="n">
-        <v>992.96</v>
+        <v>2176.01</v>
       </c>
       <c r="L36" s="1" t="n">
-        <v>1002.96</v>
+        <v>2176.01</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="N36" s="1" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="P36" s="1" t="n">
         <v>1</v>
@@ -2133,14 +2112,14 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2155,19 +2134,19 @@
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="n">
-        <v>63.52</v>
+        <v>1348.27</v>
       </c>
       <c r="L37" s="1" t="n">
-        <v>63.52</v>
+        <v>1348.27</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>78</v>
       </c>
       <c r="N37" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="P37" s="1" t="n">
         <v>1</v>
@@ -2176,14 +2155,14 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2198,13 +2177,13 @@
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1" t="n">
-        <v>63.52</v>
+        <v>1536.32</v>
       </c>
       <c r="L38" s="1" t="n">
-        <v>63.52</v>
+        <v>1536.32</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N38" s="1" t="n">
         <v>2</v>
@@ -2213,20 +2192,20 @@
         <v>34</v>
       </c>
       <c r="P38" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2241,28 +2220,28 @@
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="n">
-        <v>2176.01</v>
+        <v>1257.49</v>
       </c>
       <c r="L39" s="1" t="n">
-        <v>2176.01</v>
+        <v>1267.49</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N39" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P39" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="n">
@@ -2284,19 +2263,19 @@
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="n">
-        <v>1348.27</v>
+        <v>1589.29</v>
       </c>
       <c r="L40" s="1" t="n">
-        <v>1348.27</v>
+        <v>1589.29</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="N40" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P40" s="1" t="n">
         <v>1</v>
@@ -2305,7 +2284,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="n">
@@ -2327,19 +2306,19 @@
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="n">
-        <v>1536.32</v>
+        <v>2600.42</v>
       </c>
       <c r="L41" s="1" t="n">
-        <v>1536.32</v>
+        <v>2610.42</v>
       </c>
       <c r="M41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O41" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="N41" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="P41" s="1" t="n">
         <v>4</v>
@@ -2348,7 +2327,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="n">
@@ -2370,35 +2349,35 @@
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1" t="n">
-        <v>1257.49</v>
+        <v>916.46</v>
       </c>
       <c r="L42" s="1" t="n">
-        <v>1267.49</v>
+        <v>936.46</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N42" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="P42" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2413,19 +2392,19 @@
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="n">
-        <v>1589.29</v>
+        <v>831.19</v>
       </c>
       <c r="L43" s="1" t="n">
-        <v>1589.29</v>
+        <v>841.19</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N43" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P43" s="1" t="n">
         <v>1</v>
@@ -2434,14 +2413,14 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2456,10 +2435,10 @@
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="n">
-        <v>2600.42</v>
+        <v>1666.14</v>
       </c>
       <c r="L44" s="1" t="n">
-        <v>2610.42</v>
+        <v>1676.14</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>88</v>
@@ -2468,16 +2447,16 @@
         <v>2</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P44" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="n">
@@ -2499,19 +2478,19 @@
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1" t="n">
-        <v>916.46</v>
+        <v>2109.06</v>
       </c>
       <c r="L45" s="1" t="n">
-        <v>936.46</v>
+        <v>2109.06</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="N45" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="P45" s="1" t="n">
         <v>1</v>
@@ -2520,14 +2499,14 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2542,19 +2521,19 @@
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1" t="n">
-        <v>831.19</v>
+        <v>1481.6</v>
       </c>
       <c r="L46" s="1" t="n">
-        <v>841.19</v>
+        <v>1481.6</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="N46" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P46" s="1" t="n">
         <v>1</v>
@@ -2563,7 +2542,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="n">
@@ -2585,19 +2564,19 @@
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1" t="n">
-        <v>1666.14</v>
+        <v>679.74</v>
       </c>
       <c r="L47" s="1" t="n">
-        <v>1676.14</v>
+        <v>679.74</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N47" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P47" s="1" t="n">
         <v>1</v>
@@ -2606,7 +2585,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="n">
@@ -2628,35 +2607,35 @@
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1" t="n">
-        <v>2109.06</v>
+        <v>618.18</v>
       </c>
       <c r="L48" s="1" t="n">
-        <v>2109.06</v>
+        <v>618.18</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="N48" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P48" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2671,19 +2650,19 @@
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1" t="n">
-        <v>1481.6</v>
+        <v>618.18</v>
       </c>
       <c r="L49" s="1" t="n">
-        <v>1481.6</v>
+        <v>618.18</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="N49" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="P49" s="1" t="n">
         <v>1</v>
@@ -2692,14 +2671,14 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2714,28 +2693,28 @@
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1" t="n">
-        <v>679.74</v>
+        <v>15.41</v>
       </c>
       <c r="L50" s="1" t="n">
-        <v>679.74</v>
+        <v>15.41</v>
       </c>
       <c r="M50" s="1" t="s">
         <v>98</v>
       </c>
       <c r="N50" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="P50" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="n">
@@ -2757,35 +2736,35 @@
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1" t="n">
-        <v>618.18</v>
+        <v>13.83</v>
       </c>
       <c r="L51" s="1" t="n">
-        <v>618.18</v>
+        <v>13.83</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="N51" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P51" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2800,28 +2779,28 @@
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1" t="n">
-        <v>618.18</v>
+        <v>13.83</v>
       </c>
       <c r="L52" s="1" t="n">
-        <v>618.18</v>
+        <v>13.83</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>101</v>
       </c>
       <c r="N52" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="P52" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="n">
@@ -2843,35 +2822,35 @@
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1" t="n">
-        <v>15.41</v>
+        <v>13.83</v>
       </c>
       <c r="L53" s="1" t="n">
-        <v>15.41</v>
+        <v>13.83</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>101</v>
       </c>
       <c r="N53" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P53" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="n">
         <v>9982</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2886,19 +2865,19 @@
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1" t="n">
-        <v>13.83</v>
+        <v>609.89</v>
       </c>
       <c r="L54" s="1" t="n">
-        <v>13.83</v>
+        <v>609.89</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N54" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="P54" s="1" t="n">
         <v>1</v>
@@ -2914,12 +2893,12 @@
         <v>9982</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H55" s="1" t="n">
         <v>2</v>
@@ -2929,22 +2908,22 @@
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1" t="n">
-        <v>13.83</v>
+        <v>1009.67</v>
       </c>
       <c r="L55" s="1" t="n">
-        <v>13.83</v>
+        <v>1009.67</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="N55" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="P55" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q55" s="1"/>
     </row>
@@ -2957,7 +2936,7 @@
         <v>9982</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -2972,22 +2951,22 @@
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1" t="n">
-        <v>13.83</v>
+        <v>604.5</v>
       </c>
       <c r="L56" s="1" t="n">
-        <v>13.83</v>
+        <v>604.5</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="N56" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="P56" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q56" s="1"/>
     </row>
@@ -3015,22 +2994,22 @@
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1" t="n">
-        <v>609.89</v>
+        <v>1029.5</v>
       </c>
       <c r="L57" s="1" t="n">
-        <v>609.89</v>
+        <v>1029.5</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="N57" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="P57" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q57" s="1"/>
     </row>
@@ -3058,22 +3037,22 @@
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1" t="n">
-        <v>1009.67</v>
+        <v>1014.28</v>
       </c>
       <c r="L58" s="1" t="n">
-        <v>1009.67</v>
+        <v>1014.28</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="N58" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="P58" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q58" s="1"/>
     </row>
@@ -3101,22 +3080,22 @@
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1" t="n">
-        <v>604.5</v>
+        <v>0</v>
       </c>
       <c r="L59" s="1" t="n">
-        <v>604.5</v>
+        <v>10</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N59" s="1" t="n">
         <v>1</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="P59" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q59" s="1"/>
     </row>
@@ -3126,10 +3105,10 @@
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="n">
-        <v>9982</v>
+        <v>9983</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3140,118 +3119,108 @@
         <v>2</v>
       </c>
       <c r="I60" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1" t="n">
-        <v>1029.5</v>
+        <v>3174.49</v>
       </c>
       <c r="L60" s="1" t="n">
-        <v>1029.5</v>
+        <v>3194.49</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="N60" s="1" t="n">
         <v>1</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P60" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="n">
-        <v>9982</v>
+        <v>9984</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H61" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I61" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1" t="n">
-        <v>1014.28</v>
+        <v>706.25</v>
       </c>
       <c r="L61" s="1" t="n">
-        <v>1014.28</v>
+        <v>726.25</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N61" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="N61" s="1"/>
       <c r="O61" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P61" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="n">
-        <v>9982</v>
+        <v>9985</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H62" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I62" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1" t="n">
-        <v>0</v>
+        <v>518.75</v>
       </c>
       <c r="L62" s="1" t="n">
-        <v>10</v>
+        <v>538.75</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N62" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="N62" s="1"/>
       <c r="O62" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P62" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="n">
@@ -3263,7 +3232,7 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="H63" s="1" t="n">
         <v>2</v>
@@ -3271,42 +3240,40 @@
       <c r="I63" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="J63" s="1"/>
       <c r="K63" s="1" t="n">
-        <v>3174.49</v>
+        <v>583.25</v>
       </c>
       <c r="L63" s="1" t="n">
-        <v>3194.49</v>
+        <v>603.25</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="N63" s="1" t="n">
         <v>1</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="n">
-        <v>9984</v>
+        <v>9983</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H64" s="1" t="n">
         <v>2</v>
@@ -3314,40 +3281,40 @@
       <c r="I64" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="J64" s="1"/>
       <c r="K64" s="1" t="n">
-        <v>706.25</v>
+        <v>583.25</v>
       </c>
       <c r="L64" s="1" t="n">
-        <v>726.25</v>
+        <v>603.25</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N64" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="N64" s="1" t="n">
+        <v>33</v>
+      </c>
       <c r="O64" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="n">
-        <v>9985</v>
+        <v>9983</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H65" s="1" t="n">
         <v>2</v>
@@ -3355,40 +3322,42 @@
       <c r="I65" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J65" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="J65" s="1"/>
       <c r="K65" s="1" t="n">
-        <v>518.75</v>
+        <v>583.25</v>
       </c>
       <c r="L65" s="1" t="n">
-        <v>538.75</v>
+        <v>603.25</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N65" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="N65" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="O65" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P65" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="P65" s="1" t="n">
+        <v>34</v>
+      </c>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="n">
-        <v>9983</v>
+        <v>9984</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="H66" s="1" t="n">
         <v>2</v>
@@ -3396,197 +3365,65 @@
       <c r="I66" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J66" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="J66" s="1"/>
       <c r="K66" s="1" t="n">
-        <v>583.25</v>
+        <v>3185.66</v>
       </c>
       <c r="L66" s="1" t="n">
-        <v>603.25</v>
+        <v>3205.66</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N66" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="N66" s="1"/>
       <c r="O66" s="1" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="n">
-        <v>9983</v>
+        <v>9982</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="H67" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I67" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J67" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J67" s="1"/>
       <c r="K67" s="1" t="n">
-        <v>583.25</v>
+        <v>3465.65</v>
       </c>
       <c r="L67" s="1" t="n">
-        <v>603.25</v>
+        <v>3485.65</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N67" s="1" t="n">
-        <v>33</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="N67" s="1"/>
       <c r="O67" s="1" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1" t="n">
-        <v>9983</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H68" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I68" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K68" s="1" t="n">
-        <v>583.25</v>
-      </c>
-      <c r="L68" s="1" t="n">
-        <v>603.25</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N68" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="O68" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P68" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="Q68" s="1"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1" t="n">
-        <v>9984</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="H69" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I69" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K69" s="1" t="n">
-        <v>3185.66</v>
-      </c>
-      <c r="L69" s="1" t="n">
-        <v>3205.66</v>
-      </c>
-      <c r="M69" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1" t="n">
-        <v>9982</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H70" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I70" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K70" s="1" t="n">
-        <v>3465.65</v>
-      </c>
-      <c r="L70" s="1" t="n">
-        <v>3485.65</v>
-      </c>
-      <c r="M70" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>